<commit_message>
Implemented data driven concept
</commit_message>
<xml_diff>
--- a/OpticoTest/src/main/java/com/optico/qa/testdata/TestData.xlsx
+++ b/OpticoTest/src/main/java/com/optico/qa/testdata/TestData.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakas\learning\Optico\OpticoTest\OpticoTest\src\main\java\com\optico\qa\util\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aakas\learning\Optico\OpticoTest\OpticoTest\src\main\java\com\optico\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E3CAB4-5980-489B-93A8-3AEA1E150D6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4B4E64-336C-457F-B0FB-9151F2D252B0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="CustomerDetails" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>